<commit_message>
fixed 490 issue, created plots and figs for PPT area
</commit_message>
<xml_diff>
--- a/Paper2/isotherms.xlsx
+++ b/Paper2/isotherms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marijailoska/Desktop/CO_Pd/Paper2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1580DBC7-BB24-4746-AE61-45F854F883FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF36BCA-24BF-E94D-847C-D5628C7E70B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="25340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coverage vs Wavenumber" sheetId="6" r:id="rId1"/>
@@ -1357,7 +1357,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Data combined'!$K$3:$K$9</c15:sqref>
@@ -1393,7 +1393,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Data combined'!$AG$3:$AG$9</c15:sqref>
@@ -1428,7 +1428,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-7391-4AE4-B676-C8F830C92C83}"/>
                   </c:ext>
@@ -1482,7 +1482,7 @@
                   </c:numLit>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-7391-4AE4-B676-C8F830C92C83}"/>
                   </c:ext>
@@ -2656,7 +2656,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Data combined'!$K$1</c15:sqref>
@@ -2697,7 +2697,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Data combined'!$J$3:$J$10</c15:sqref>
@@ -2736,7 +2736,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Data combined'!$K$3:$K$10</c15:sqref>
@@ -2771,7 +2771,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="1"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-66ED-4809-9F97-8879349A0478}"/>
                   </c:ext>
@@ -4253,6 +4253,640 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>450 K</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data combined'!$O$3:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9999999999999998E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999995E-8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9999999999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0000000000000004E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data combined'!$P$3:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1830.1546599999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1834.0116800000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1861.0108</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1872.58185</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1891.8669400000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1897.65246</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-23C2-9E4E-A99E-174D4AEB2708}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>490 K</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data combined'!$V$3:$V$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1499999999999998E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1999999999999999E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9999999999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data combined'!$W$3:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1812.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1818.58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1820.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1824.37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1834</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1855.23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1864.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-23C2-9E4E-A99E-174D4AEB2708}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>475 K</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data combined'!$AF$3:$AF$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.3000000000000001E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2000000000000002E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1600000000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8599999999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7600000000000006E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3759999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0976E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data combined'!$AG$3:$AG$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1814.73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1820.51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1820.51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1839.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1843.65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1874.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1882.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-23C2-9E4E-A99E-174D4AEB2708}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1862009120"/>
+        <c:axId val="1862010672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1862009120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Pressure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1862010672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1862010672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Wavenumber</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1862009120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:overlay val="0"/>
       <c:spPr>
@@ -5631,6 +6265,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7695,11 +8369,527 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9B156276-9C72-44BF-B830-2B65EF3247FD}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="209" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7710,7 +8900,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{195E14AF-4E65-4FDF-AC1C-ACE9B93CFB94}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="209" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7721,7 +8911,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659628" cy="6279116"/>
+    <xdr:ext cx="8676640" cy="6289040"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8116,7 +9306,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659628" cy="6279116"/>
+    <xdr:ext cx="8677321" cy="6289234"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8830,6 +10020,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>279423</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>14934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>381625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>125123</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D70920F-3001-8588-D347-8D9470746A1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9459,23 +10685,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F85F3B6-CECE-4796-AC18-311CECB623C1}">
   <dimension ref="A1:AJ29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3:W9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="16.296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.296875" customWidth="1"/>
-    <col min="18" max="18" width="20.09765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.8984375" customWidth="1"/>
-    <col min="24" max="24" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="18" max="18" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" customWidth="1"/>
+    <col min="24" max="24" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -9520,7 +10746,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9588,7 +10814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1.2623810779268201E-8</v>
       </c>
@@ -9659,7 +10885,7 @@
         <v>3.0072000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>7.4989420933245495E-8</v>
       </c>
@@ -9730,7 +10956,7 @@
         <v>8.2005000000000008E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2.4040991835099699E-7</v>
       </c>
@@ -9801,7 +11027,7 @@
         <v>0.13713</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>8.4834289824407198E-7</v>
       </c>
@@ -9872,7 +11098,7 @@
         <v>0.23499</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2.0961799924531201E-6</v>
       </c>
@@ -9943,7 +11169,7 @@
         <v>0.28415100000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7.9215382540609097E-6</v>
       </c>
@@ -10014,7 +11240,7 @@
         <v>0.36792000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>2.5395800383208298E-5</v>
       </c>
@@ -10079,7 +11305,7 @@
         <v>0.38262000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="E10">
         <v>3.4333200182819897E-5</v>
       </c>
@@ -10135,7 +11361,7 @@
         <v>0.40454400000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="O11" s="1">
@@ -10152,7 +11378,7 @@
         <v>0.40085490342953001</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="O12" s="1">
@@ -10169,7 +11395,7 @@
         <v>0.36315711829412001</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -10189,7 +11415,7 @@
         <v>0.22367711736996448</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -10207,7 +11433,7 @@
         <v>5.2760736196317388E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1.30388850284448E-2</v>
       </c>
@@ -10224,7 +11450,7 @@
         <v>5.2760736196317388E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2.9151625058612799E-2</v>
       </c>
@@ -10245,7 +11471,7 @@
         <v>0.10828220858895675</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>5.8573857826438203E-2</v>
       </c>
@@ -10262,7 +11488,7 @@
         <v>0.15030674846625763</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8.09919269641656E-2</v>
       </c>
@@ -10283,7 +11509,7 @@
         <v>0.22730061349693201</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>9.4303114530899596E-2</v>
       </c>
@@ -10300,7 +11526,7 @@
         <v>0.26395705521472346</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.121633928218339</v>
       </c>
@@ -10321,7 +11547,7 @@
         <v>0.34432515337423297</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.18187832257116801</v>
       </c>
@@ -10338,7 +11564,7 @@
         <v>0.371932515337423</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.24072561282194599</v>
       </c>
@@ -10356,7 +11582,7 @@
         <v>0.26395705521472346</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.29752780932042999</v>
       </c>
@@ -10370,7 +11596,7 @@
         <v>0.17607361963190099</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.31924873876469501</v>
       </c>
@@ -10388,7 +11614,7 @@
         <v>0.34432515337423297</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.409326644407911</v>
       </c>
@@ -10402,7 +11628,7 @@
         <v>0.28343558282208597</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.41921653701224199</v>
       </c>
@@ -10420,7 +11646,7 @@
         <v>0.371932515337423</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0.45080193662469098</v>
       </c>
@@ -10434,7 +11660,7 @@
         <v>0.32177914110429401</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0.478862091758046</v>
       </c>
@@ -10442,7 +11668,7 @@
         <v>1938.33330508618</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.50552344796027304</v>
       </c>
@@ -10468,12 +11694,12 @@
       <selection activeCell="A7" sqref="A7:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
         <v>8.4834289824407195E-8</v>
       </c>
@@ -10496,7 +11722,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>4.0470899507597598E-7</v>
       </c>
@@ -10516,7 +11742,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>9.2105531768948098E-7</v>
       </c>
@@ -10536,7 +11762,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>4.1029406807469902E-6</v>
       </c>
@@ -10556,7 +11782,7 @@
         <v>1.28504672897196E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1.24519708473503E-5</v>
       </c>
@@ -10570,7 +11796,7 @@
         <v>0.15070093000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3.9376589235643897E-5</v>
       </c>
@@ -10584,7 +11810,7 @@
         <v>6.6588785046728896E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1.5085907086001701E-8</v>
       </c>
@@ -10595,7 +11821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>3.62680169079641E-8</v>
       </c>
@@ -10603,7 +11829,7 @@
         <v>1.28504672897196E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8.7191909835962602E-8</v>
       </c>
@@ -10611,7 +11837,7 @@
         <v>4.2056074766354999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2.7953009456081902E-7</v>
       </c>
@@ -10619,7 +11845,7 @@
         <v>0.101635514018691</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8.0308572213915202E-7</v>
       </c>
@@ -10627,7 +11853,7 @@
         <v>0.16355140186915801</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2.4040991835099698E-6</v>
       </c>
@@ -10635,7 +11861,7 @@
         <v>0.23481308411214899</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>8.60050216520387E-6</v>
       </c>
@@ -10643,7 +11869,7 @@
         <v>0.309579439252336</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3.4333200182819897E-5</v>
       </c>
@@ -10651,7 +11877,7 @@
         <v>0.37383177570093401</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1.2623810779268201E-8</v>
       </c>
@@ -10662,7 +11888,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>7.4989420933245495E-8</v>
       </c>
@@ -10670,7 +11896,7 @@
         <v>0.217289719626168</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2.4040991835099699E-7</v>
       </c>
@@ -10678,7 +11904,7 @@
         <v>0.28621495327102803</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>8.4834289824407198E-7</v>
       </c>
@@ -10686,7 +11912,7 @@
         <v>0.34579439252336402</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2.0961799924531201E-6</v>
       </c>
@@ -10694,7 +11920,7 @@
         <v>0.37850467289719603</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>7.9215382540609097E-6</v>
       </c>
@@ -10702,7 +11928,7 @@
         <v>0.414719626168224</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>2.5395800383208298E-5</v>
       </c>
@@ -10710,7 +11936,7 @@
         <v>0.43808411214953202</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1.6155980984398698E-8</v>
       </c>
@@ -10721,7 +11947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>7.0022577875305695E-8</v>
       </c>
@@ -10729,7 +11955,7 @@
         <v>0.22546728971962601</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>3.3404849835132402E-7</v>
       </c>
@@ -10737,7 +11963,7 @@
         <v>0.31658878504672899</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>8.6005021652038704E-7</v>
       </c>
@@ -10745,7 +11971,7 @@
         <v>0.35864485981308403</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2.0676460233142298E-6</v>
       </c>
@@ -10753,7 +11979,7 @@
         <v>0.39018691588784998</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>7.29617493318347E-6</v>
       </c>
@@ -10761,7 +11987,7 @@
         <v>0.42523364485981302</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>1.05635410374918E-8</v>
       </c>
@@ -10772,7 +11998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>3.8311868495572802E-8</v>
       </c>
@@ -10780,7 +12006,7 @@
         <v>0.30841121495327101</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>1.2115276586285901E-7</v>
       </c>
@@ -10788,7 +12014,7 @@
         <v>0.35864485981308403</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>4.5784058278544102E-7</v>
       </c>
@@ -10796,7 +12022,7 @@
         <v>0.407710280373831</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>9.2105531768948098E-7</v>
       </c>
@@ -10804,7 +12030,7 @@
         <v>0.42640186915887801</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>2.21430833722479E-6</v>
       </c>
@@ -10812,7 +12038,7 @@
         <v>0.44275700934579398</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>7.29617493318347E-6</v>
       </c>
@@ -10820,7 +12046,7 @@
         <v>0.45794392523364402</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>2.2758459260747899E-5</v>
       </c>
@@ -10828,7 +12054,7 @@
         <v>0.46845794392523299</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>1.3153690504363701E-8</v>
       </c>
@@ -10839,7 +12065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>9.4665226030818996E-8</v>
       </c>
@@ -10847,7 +12073,7 @@
         <v>0.38668224299065401</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2.7953009456081902E-7</v>
       </c>
@@ -10855,7 +12081,7 @@
         <v>0.41588785046728899</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>8.2540418526801701E-7</v>
       </c>
@@ -10863,7 +12089,7 @@
         <v>0.43808411214953202</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2.6826957952797202E-6</v>
       </c>
@@ -10871,7 +12097,7 @@
         <v>0.45794392523364402</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>8.3679494426834103E-6</v>
       </c>
@@ -10879,7 +12105,7 @@
         <v>0.46845794392523299</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>2.4040991835099699E-8</v>
       </c>
@@ -10890,7 +12116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>9.3376608332045502E-8</v>
       </c>
@@ -10898,7 +12124,7 @@
         <v>0.42406542056074698</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>2.43727628013851E-7</v>
       </c>
@@ -10906,7 +12132,7 @@
         <v>0.44392523364485897</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>8.1416848144757198E-7</v>
       </c>
@@ -10914,7 +12140,7 @@
         <v>0.46261682242990598</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>2.4709112279856E-6</v>
       </c>
@@ -10922,7 +12148,7 @@
         <v>0.47546728971962599</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>8.0308572213915192E-6</v>
       </c>
@@ -10930,7 +12156,7 @@
         <v>0.48247663551401798</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>1.04197462512395E-8</v>
       </c>
@@ -10941,7 +12167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2.01173804228079E-8</v>
       </c>
@@ -10949,7 +12175,7 @@
         <v>0.42873831775700899</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>6.2750768310550399E-8</v>
       </c>
@@ -10957,7 +12183,7 @@
         <v>0.45327102803738301</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2.01173804228079E-7</v>
       </c>
@@ -10965,7 +12191,7 @@
         <v>0.46845794392523299</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>6.53847082866259E-7</v>
       </c>
@@ -10973,7 +12199,7 @@
         <v>0.47546728971962599</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2.4709112279856E-6</v>
       </c>
@@ -10981,7 +12207,7 @@
         <v>0.48247663551401798</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>8.0308572213915192E-6</v>
       </c>
@@ -10989,7 +12215,7 @@
         <v>0.48831775700934499</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>1.02779088522383E-8</v>
       </c>
@@ -11000,7 +12226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>3.0348893187223099E-8</v>
       </c>
@@ -11008,7 +12234,7 @@
         <v>0.46845794392523299</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>9.0851757565168603E-8</v>
       </c>
@@ -11016,7 +12242,7 @@
         <v>0.47663551401869098</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>2.1544346900318801E-7</v>
       </c>
@@ -11024,7 +12250,7 @@
         <v>0.48247663551401798</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>6.9069404921020798E-7</v>
       </c>
@@ -11032,7 +12258,7 @@
         <v>0.48714953271028</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>2.2758459260747899E-6</v>
       </c>
@@ -11040,7 +12266,7 @@
         <v>0.49182242990654201</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>8.0308572213915192E-6</v>
       </c>
@@ -11048,7 +12274,7 @@
         <v>0.49415887850467199</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>1.7066436812963402E-8</v>
       </c>
@@ -11059,7 +12285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>8.0308572213915197E-8</v>
       </c>
@@ -11067,7 +12293,7 @@
         <v>0.49883177570093401</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>3.5287350208467498E-7</v>
       </c>
@@ -11075,7 +12301,7 @@
         <v>0.49649532710280297</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>9.9999999999999995E-7</v>
       </c>

</xml_diff>